<commit_message>
Checklist(2 versions), change to document Test design
</commit_message>
<xml_diff>
--- a/Test design/Equivalent breakdown and analysis of boundary values/ID1.xlsx
+++ b/Test design/Equivalent breakdown and analysis of boundary values/ID1.xlsx
@@ -93,11 +93,11 @@
     <t>Спец символы</t>
   </si>
   <si>
-    <t>0 - 7 символов, включая минимум 
+    <t>1 - 7 символов, включая минимум 
 одну латинскую букву и одну цифру.</t>
   </si>
   <si>
-    <t>0,1, 6, 7, 8</t>
+    <t>1, 6, 7, 8</t>
   </si>
 </sst>
 </file>
@@ -1260,7 +1260,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1"/>
@@ -1356,7 +1356,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1"/>

</xml_diff>

<commit_message>
Add change to ID1 (Equivalent breakdown and analysis of boundary values)
</commit_message>
<xml_diff>
--- a/Test design/Equivalent breakdown and analysis of boundary values/ID1.xlsx
+++ b/Test design/Equivalent breakdown and analysis of boundary values/ID1.xlsx
@@ -1260,7 +1260,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A1" sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1"/>
@@ -1356,7 +1356,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A1" sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="1"/>

</xml_diff>